<commit_message>
Added results and organized discussion
</commit_message>
<xml_diff>
--- a/Monk-manuscript/reef_areas.xlsx
+++ b/Monk-manuscript/reef_areas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20390"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\melissa.monk\Documents\GitHub\habitat-indices-paper\Monk-manuscript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF401DD9-3ECC-4394-BEF1-480AF715CBDB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B9541B2-DFA1-49C4-9368-9DA50C73BE20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19580" windowHeight="7230" xr2:uid="{50D88F75-490B-4A1E-A3D3-96979C9DECCF}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t xml:space="preserve"> Morro Bay to Point Conception </t>
   </si>
   <si>
-    <t xml:space="preserve"> Deeper rocky habitat </t>
-  </si>
-  <si>
     <t>China rockfish</t>
   </si>
   <si>
@@ -61,6 +58,9 @@
   </si>
   <si>
     <t xml:space="preserve"> California border to San Francisco</t>
+  </si>
+  <si>
+    <t>Farallon Islands</t>
   </si>
 </sst>
 </file>
@@ -416,11 +416,12 @@
   <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B9" sqref="B9:B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
+    <col min="1" max="1" width="29.7265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22.6328125" customWidth="1"/>
     <col min="3" max="3" width="13.08984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.26953125" bestFit="1" customWidth="1"/>
@@ -433,7 +434,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
@@ -442,7 +443,7 @@
         <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
@@ -450,7 +451,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>439.54599999999999</v>
@@ -469,7 +470,7 @@
       </c>
       <c r="F2">
         <f>SUM($B$2:$B$5)</f>
-        <v>685.57299999999998</v>
+        <v>735.82500000000005</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -484,40 +485,40 @@
         <v>108.42400000000001</v>
       </c>
       <c r="D3">
-        <f>SUM(B3,B4)</f>
-        <v>158.67600000000002</v>
+        <f>$C$3+$C$4</f>
+        <v>498.96699999999998</v>
       </c>
       <c r="E3">
         <f>B2+B3</f>
         <v>547.97</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F5" si="1">SUM($B$2:$B$5)</f>
-        <v>685.57299999999998</v>
+        <f>SUM($B$2:$B$5)</f>
+        <v>735.82500000000005</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4">
         <v>50.252000000000002</v>
       </c>
       <c r="C4" s="1">
         <f>SUM($B$4:$B$7)</f>
-        <v>340.291</v>
+        <v>390.54300000000001</v>
       </c>
       <c r="D4">
-        <f>D3</f>
-        <v>158.67600000000002</v>
+        <f>$C$3+$C$4</f>
+        <v>498.96699999999998</v>
       </c>
       <c r="E4">
         <f>B4</f>
         <v>50.252000000000002</v>
       </c>
       <c r="F4">
-        <f t="shared" si="1"/>
-        <v>685.57299999999998</v>
+        <f t="shared" ref="F4:F5" si="1">SUM($B$2:$B$5)</f>
+        <v>735.82500000000005</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -525,23 +526,23 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>87.350999999999999</v>
+        <v>137.60300000000001</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:C7" si="2">SUM($B$4:$B$7)</f>
-        <v>340.291</v>
+        <f>SUM($B$4:$B$7)</f>
+        <v>390.54300000000001</v>
       </c>
       <c r="D5">
         <f>SUM($B$5:$B$6)</f>
-        <v>177.77500000000001</v>
+        <v>228.02700000000002</v>
       </c>
       <c r="E5">
         <f>B5</f>
-        <v>87.350999999999999</v>
+        <v>137.60300000000001</v>
       </c>
       <c r="F5">
         <f t="shared" si="1"/>
-        <v>685.57299999999998</v>
+        <v>735.82500000000005</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -552,12 +553,12 @@
         <v>90.424000000000007</v>
       </c>
       <c r="C6" s="1">
-        <f t="shared" si="2"/>
-        <v>340.291</v>
+        <f t="shared" ref="C6:C7" si="2">SUM($B$4:$B$7)</f>
+        <v>390.54300000000001</v>
       </c>
       <c r="D6">
         <f>SUM($B$5:$B$6)</f>
-        <v>177.77500000000001</v>
+        <v>228.02700000000002</v>
       </c>
       <c r="E6">
         <f>B6+B7</f>
@@ -577,7 +578,7 @@
       </c>
       <c r="C7" s="1">
         <f t="shared" si="2"/>
-        <v>340.291</v>
+        <v>390.54300000000001</v>
       </c>
       <c r="D7">
         <f>B7</f>

</xml_diff>